<commit_message>
test/perl_output/formats.xlsx : regenerate by excel-writer-xlsx 0.49
</commit_message>
<xml_diff>
--- a/test/perl_output/formats.xlsx
+++ b/test/perl_output/formats.xlsx
@@ -1125,8 +1125,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
     <fill>

</xml_diff>

<commit_message>
If cell format is force text (49=>'@'), then worksheet#write will write a string.
</commit_message>
<xml_diff>
--- a/test/perl_output/formats.xlsx
+++ b/test/perl_output/formats.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="187">
   <si>
     <t>This workbook demonstrates some of</t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t>##0.0E+0</t>
+  </si>
+  <si>
+    <t>1234.567</t>
   </si>
   <si>
     <t>@</t>
@@ -3766,11 +3769,11 @@
       <c r="C37" s="20">
         <v>1234.567</v>
       </c>
-      <c r="D37" s="112">
-        <v>1234.567</v>
+      <c r="D37" s="112" t="s">
+        <v>149</v>
       </c>
       <c r="F37" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3798,15 +3801,15 @@
         <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="F2" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3817,7 +3820,7 @@
         <v>106</v>
       </c>
       <c r="D3" s="113" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3828,7 +3831,7 @@
         <v>108</v>
       </c>
       <c r="D5" s="114" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3839,7 +3842,7 @@
         <v>110</v>
       </c>
       <c r="D7" s="115" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3850,7 +3853,7 @@
         <v>112</v>
       </c>
       <c r="D9" s="116" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3861,7 +3864,7 @@
         <v>114</v>
       </c>
       <c r="D11" s="117" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3872,7 +3875,7 @@
         <v>116</v>
       </c>
       <c r="D13" s="118" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3883,7 +3886,7 @@
         <v>118</v>
       </c>
       <c r="D15" s="119" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3894,7 +3897,7 @@
         <v>120</v>
       </c>
       <c r="D17" s="120" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3905,7 +3908,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="121" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3916,7 +3919,7 @@
         <v>48</v>
       </c>
       <c r="D21" s="122" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3927,7 +3930,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="123" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3938,7 +3941,7 @@
         <v>32</v>
       </c>
       <c r="D25" s="124" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3949,7 +3952,7 @@
         <v>50</v>
       </c>
       <c r="D27" s="125" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3960,21 +3963,21 @@
         <v>42</v>
       </c>
       <c r="D29" s="126" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3985,7 +3988,7 @@
         <v>108</v>
       </c>
       <c r="D33" s="127" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3996,7 +3999,7 @@
         <v>110</v>
       </c>
       <c r="D35" s="128" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -4007,7 +4010,7 @@
         <v>112</v>
       </c>
       <c r="D37" s="129" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4035,15 +4038,15 @@
         <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="F2" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4054,7 +4057,7 @@
         <v>106</v>
       </c>
       <c r="D3" s="130" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4065,10 +4068,10 @@
         <v>108</v>
       </c>
       <c r="D5" s="131" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4079,7 +4082,7 @@
         <v>110</v>
       </c>
       <c r="D7" s="132" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4090,7 +4093,7 @@
         <v>112</v>
       </c>
       <c r="D9" s="133" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -4101,7 +4104,7 @@
         <v>114</v>
       </c>
       <c r="D11" s="134" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -4112,7 +4115,7 @@
         <v>116</v>
       </c>
       <c r="D13" s="135" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -4123,7 +4126,7 @@
         <v>118</v>
       </c>
       <c r="D15" s="136" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4134,7 +4137,7 @@
         <v>120</v>
       </c>
       <c r="D17" s="137" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4145,7 +4148,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="138" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4156,7 +4159,7 @@
         <v>48</v>
       </c>
       <c r="D21" s="139" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4167,7 +4170,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="140" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4178,7 +4181,7 @@
         <v>32</v>
       </c>
       <c r="D25" s="141" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -4189,7 +4192,7 @@
         <v>50</v>
       </c>
       <c r="D27" s="142" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4200,7 +4203,7 @@
         <v>42</v>
       </c>
       <c r="D29" s="143" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -4211,7 +4214,7 @@
         <v>54</v>
       </c>
       <c r="D31" s="144" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -4222,7 +4225,7 @@
         <v>52</v>
       </c>
       <c r="D33" s="145" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -4233,7 +4236,7 @@
         <v>44</v>
       </c>
       <c r="D35" s="146" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -4244,7 +4247,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="147" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -4255,7 +4258,7 @@
         <v>40</v>
       </c>
       <c r="D39" s="148" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -4278,72 +4281,72 @@
   <sheetData>
     <row r="1" spans="1:6" ht="40" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B1" s="149" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C1" s="150" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D1" s="151" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E1" s="152" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F1" s="153" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B3" s="154" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C3" s="155" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E3" s="156" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F3" s="157" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" s="158" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C4" s="158"/>
       <c r="D4" s="159" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E4" s="160" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B6" s="161" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="162" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="163" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4364,37 +4367,37 @@
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" s="164" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="3:3">
       <c r="C4" s="165" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" s="166" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" s="167" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" s="168" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" s="169" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" s="170" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix handling of 'num_format': '0' in duplicate formats.
</commit_message>
<xml_diff>
--- a/test/perl_output/formats.xlsx
+++ b/test/perl_output/formats.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Alignment" sheetId="8" r:id="rId8"/>
     <sheet name="Miscellaneous" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1572,7 +1572,7 @@
     <xf numFmtId="0" fontId="0" fillId="55" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="56" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="57" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>

</xml_diff>